<commit_message>
Added PSA input file, still needs work
</commit_message>
<xml_diff>
--- a/output/PSA.xlsx
+++ b/output/PSA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="50">
   <si>
     <t>DALYs</t>
   </si>
@@ -145,6 +145,27 @@
   </si>
   <si>
     <t>I have worked with 105 million in excel, and that worked ok, so I don't expect problems there.</t>
+  </si>
+  <si>
+    <t>Diabetes Incidence</t>
+  </si>
+  <si>
+    <t>CHD Incidence</t>
+  </si>
+  <si>
+    <t>HCC Incidence</t>
+  </si>
+  <si>
+    <t>T2D incidence, CHD incidence, HCC Incidence</t>
+  </si>
+  <si>
+    <t>Prevalence states:</t>
+  </si>
+  <si>
+    <t>Events for:</t>
+  </si>
+  <si>
+    <t>Steatosis, NASH, Cirrhosis, HCC, LiverDeath, NaturalDeath, CHD, CHD death, T2D, T2D death, overweight, obesity</t>
   </si>
 </sst>
 </file>
@@ -524,17 +545,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CRQ34"/>
+  <dimension ref="A1:CRQ37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
     <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
@@ -1848,13 +1869,13 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="AD3" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="BE3" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="CF3" t="s">
         <v>1</v>
@@ -2128,7 +2149,7 @@
       </c>
     </row>
     <row r="4" spans="1:2513" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C4">
@@ -10108,14 +10129,30 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>